<commit_message>
add polyp numbers and comments
</commit_message>
<xml_diff>
--- a/respirometry_info.xlsx
+++ b/respirometry_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amelia/github/MHWsim-respo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DEFABE7-4A3C-E545-BBEF-9E487716A3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041A1D0B-1665-8144-BFFE-16ADB97B9ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="500" windowWidth="17720" windowHeight="19480" xr2:uid="{E6A47E57-F094-2D4A-9291-917180B3F4AD}"/>
+    <workbookView xWindow="940" yWindow="500" windowWidth="22540" windowHeight="19480" xr2:uid="{E6A47E57-F094-2D4A-9291-917180B3F4AD}"/>
   </bookViews>
   <sheets>
     <sheet name="run info" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,36 @@
   </si>
   <si>
     <t>or 4 polyps?</t>
+  </si>
+  <si>
+    <t>actually 7 polyps but removed 2 tiny maybe</t>
+  </si>
+  <si>
+    <t>labeled tube (2)</t>
+  </si>
+  <si>
+    <t>Give it 1 hour to temperature stabilize</t>
+  </si>
+  <si>
+    <t>Give it 1 hour to temperature stabilize; Only 6 polyps frozen</t>
+  </si>
+  <si>
+    <t>Either E7 or E10 has one of the frozen vials labeled "12/10/23" on the top cap (but it should be 12/12)</t>
+  </si>
+  <si>
+    <t>vial labeled b</t>
+  </si>
+  <si>
+    <t>vial labeled b; poorly labeled vial</t>
+  </si>
+  <si>
+    <t>vial labeled C12 but it is C11, and the second vial is 4 polyps not 1 polyp</t>
+  </si>
+  <si>
+    <t>vial not labeled b!!</t>
+  </si>
+  <si>
+    <t>only 1 vial for all polyps</t>
   </si>
 </sst>
 </file>
@@ -492,7 +522,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J484" sqref="J484"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4131,7 +4161,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>45269</v>
       </c>
@@ -4160,7 +4190,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>45269</v>
       </c>
@@ -4189,7 +4219,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>45269</v>
       </c>
@@ -4218,7 +4248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>45269</v>
       </c>
@@ -4247,7 +4277,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>45269</v>
       </c>
@@ -4276,7 +4306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>45269</v>
       </c>
@@ -4299,7 +4329,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>45269</v>
       </c>
@@ -4322,7 +4352,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>45269</v>
       </c>
@@ -4345,7 +4375,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
         <v>45269</v>
       </c>
@@ -4368,7 +4398,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>45269</v>
       </c>
@@ -4391,7 +4421,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
         <v>45269</v>
       </c>
@@ -4414,7 +4444,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>45270</v>
       </c>
@@ -4446,7 +4476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
         <v>45270</v>
       </c>
@@ -4478,7 +4508,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
         <v>45270</v>
       </c>
@@ -4510,7 +4540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
         <v>45270</v>
       </c>
@@ -4541,8 +4571,11 @@
       <c r="J143">
         <v>5</v>
       </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K143" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
         <v>45270</v>
       </c>
@@ -4572,6 +4605,9 @@
       </c>
       <c r="J144">
         <v>7</v>
+      </c>
+      <c r="K144" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.2">
@@ -5032,7 +5068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
         <v>45270</v>
       </c>
@@ -5055,7 +5091,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
         <v>45270</v>
       </c>
@@ -5078,7 +5114,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
         <v>45270</v>
       </c>
@@ -5101,7 +5137,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
         <v>45271</v>
       </c>
@@ -5132,8 +5168,11 @@
       <c r="J164">
         <v>3</v>
       </c>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K164" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
         <v>45271</v>
       </c>
@@ -5164,8 +5203,11 @@
       <c r="J165">
         <v>5</v>
       </c>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K165" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
         <v>45271</v>
       </c>
@@ -5196,8 +5238,11 @@
       <c r="J166">
         <v>3</v>
       </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K166" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167" s="2">
         <v>45271</v>
       </c>
@@ -5228,8 +5273,11 @@
       <c r="J167">
         <v>7</v>
       </c>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K167" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
         <v>45271</v>
       </c>
@@ -5260,8 +5308,11 @@
       <c r="J168">
         <v>7</v>
       </c>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K168" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169" s="2">
         <v>45271</v>
       </c>
@@ -5292,8 +5343,11 @@
       <c r="J169">
         <v>7</v>
       </c>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K169" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
         <v>45271</v>
       </c>
@@ -5322,7 +5376,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171" s="2">
         <v>45271</v>
       </c>
@@ -5351,7 +5405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
         <v>45271</v>
       </c>
@@ -5380,7 +5434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173" s="2">
         <v>45271</v>
       </c>
@@ -5409,7 +5463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
         <v>45271</v>
       </c>
@@ -5438,7 +5492,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175" s="2">
         <v>45271</v>
       </c>
@@ -5467,7 +5521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
         <v>45271</v>
       </c>
@@ -5799,6 +5853,9 @@
       <c r="J187">
         <v>8</v>
       </c>
+      <c r="K187" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
@@ -6391,7 +6448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A209" s="2">
         <v>45272</v>
       </c>
@@ -6420,7 +6477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A210" s="2">
         <v>45272</v>
       </c>
@@ -6449,7 +6506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A211" s="2">
         <v>45272</v>
       </c>
@@ -6478,7 +6535,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A212" s="2">
         <v>45272</v>
       </c>
@@ -6501,7 +6558,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A213" s="2">
         <v>45272</v>
       </c>
@@ -6524,7 +6581,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A214" s="2">
         <v>45272</v>
       </c>
@@ -6547,7 +6604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A215" s="2">
         <v>45272</v>
       </c>
@@ -6570,7 +6627,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A216" s="2">
         <v>45272</v>
       </c>
@@ -6593,7 +6650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A217" s="2">
         <v>45272</v>
       </c>
@@ -6616,7 +6673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A218" s="2">
         <v>45336</v>
       </c>
@@ -6648,7 +6705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A219" s="2">
         <v>45336</v>
       </c>
@@ -6680,7 +6737,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A220" s="2">
         <v>45336</v>
       </c>
@@ -6712,7 +6769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A221" s="2">
         <v>45336</v>
       </c>
@@ -6744,7 +6801,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A222" s="2">
         <v>45336</v>
       </c>
@@ -6776,7 +6833,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A223" s="2">
         <v>45336</v>
       </c>
@@ -6807,8 +6864,11 @@
       <c r="J223">
         <v>5</v>
       </c>
-    </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K223" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A224" s="2">
         <v>45336</v>
       </c>
@@ -6839,8 +6899,11 @@
       <c r="J224">
         <v>8</v>
       </c>
-    </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K224" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A225" s="2">
         <v>45336</v>
       </c>
@@ -6869,7 +6932,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A226" s="2">
         <v>45336</v>
       </c>
@@ -6898,7 +6961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A227" s="2">
         <v>45336</v>
       </c>
@@ -6927,7 +6990,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A228" s="2">
         <v>45336</v>
       </c>
@@ -6956,7 +7019,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A229" s="2">
         <v>45336</v>
       </c>
@@ -6985,7 +7048,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A230" s="2">
         <v>45336</v>
       </c>
@@ -7014,7 +7077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A231" s="2">
         <v>45336</v>
       </c>
@@ -7043,7 +7106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A232" s="2">
         <v>45336</v>
       </c>
@@ -7075,7 +7138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A233" s="2">
         <v>45336</v>
       </c>
@@ -7107,7 +7170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A234" s="2">
         <v>45336</v>
       </c>
@@ -7139,7 +7202,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A235" s="2">
         <v>45336</v>
       </c>
@@ -7171,7 +7234,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A236" s="2">
         <v>45336</v>
       </c>
@@ -7203,7 +7266,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A237" s="2">
         <v>45336</v>
       </c>
@@ -7234,8 +7297,11 @@
       <c r="J237">
         <v>6</v>
       </c>
-    </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K237" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A238" s="2">
         <v>45336</v>
       </c>
@@ -7266,8 +7332,11 @@
       <c r="J238">
         <v>6</v>
       </c>
-    </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K238" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A239" s="2">
         <v>45336</v>
       </c>
@@ -7296,7 +7365,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A240" s="2">
         <v>45336</v>
       </c>
@@ -7325,7 +7394,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A241" s="2">
         <v>45336</v>
       </c>
@@ -7354,7 +7423,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A242" s="2">
         <v>45336</v>
       </c>
@@ -7383,7 +7452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A243" s="2">
         <v>45336</v>
       </c>
@@ -7412,7 +7481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A244" s="2">
         <v>45336</v>
       </c>
@@ -7441,7 +7510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A245" s="2">
         <v>45336</v>
       </c>
@@ -7470,7 +7539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A246" s="2">
         <v>45336</v>
       </c>
@@ -7493,7 +7562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A247" s="2">
         <v>45336</v>
       </c>
@@ -7516,7 +7585,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A248" s="2">
         <v>45336</v>
       </c>
@@ -7539,7 +7608,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A249" s="2">
         <v>45336</v>
       </c>
@@ -7562,7 +7631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A250" s="2">
         <v>45336</v>
       </c>
@@ -7585,7 +7654,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A251" s="2">
         <v>45336</v>
       </c>
@@ -7608,7 +7677,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A252" s="2">
         <v>45336</v>
       </c>
@@ -7631,7 +7700,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A253" s="2">
         <v>45337</v>
       </c>
@@ -7662,8 +7731,11 @@
       <c r="J253">
         <v>5</v>
       </c>
-    </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K253" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A254" s="2">
         <v>45337</v>
       </c>
@@ -7695,7 +7767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A255" s="2">
         <v>45337</v>
       </c>
@@ -7726,8 +7798,11 @@
       <c r="J255">
         <v>4</v>
       </c>
-    </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K255" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A256" s="2">
         <v>45337</v>
       </c>
@@ -7759,7 +7834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A257" s="2">
         <v>45337</v>
       </c>
@@ -7791,7 +7866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A258" s="2">
         <v>45337</v>
       </c>
@@ -7822,8 +7897,11 @@
       <c r="J258">
         <v>7</v>
       </c>
-    </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K258" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A259" s="2">
         <v>45337</v>
       </c>
@@ -7854,8 +7932,11 @@
       <c r="J259">
         <v>3</v>
       </c>
-    </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K259" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A260" s="2">
         <v>45337</v>
       </c>
@@ -7884,7 +7965,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A261" s="2">
         <v>45337</v>
       </c>
@@ -7913,7 +7994,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A262" s="2">
         <v>45337</v>
       </c>
@@ -7942,7 +8023,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A263" s="2">
         <v>45337</v>
       </c>
@@ -7971,7 +8052,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A264" s="2">
         <v>45337</v>
       </c>
@@ -8000,7 +8081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A265" s="2">
         <v>45337</v>
       </c>
@@ -8029,7 +8110,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A266" s="2">
         <v>45337</v>
       </c>
@@ -8058,7 +8139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A267" s="2">
         <v>45337</v>
       </c>
@@ -8090,7 +8171,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A268" s="2">
         <v>45337</v>
       </c>
@@ -8122,7 +8203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A269" s="2">
         <v>45337</v>
       </c>
@@ -8154,7 +8235,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A270" s="2">
         <v>45337</v>
       </c>
@@ -8186,7 +8267,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A271" s="2">
         <v>45337</v>
       </c>
@@ -8218,7 +8299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A272" s="2">
         <v>45337</v>
       </c>
@@ -9176,7 +9257,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A305" s="2">
         <v>45338</v>
       </c>
@@ -9208,7 +9289,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A306" s="2">
         <v>45338</v>
       </c>
@@ -9239,8 +9320,11 @@
       <c r="J306" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K306" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="307" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A307" s="2">
         <v>45338</v>
       </c>
@@ -9272,7 +9356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A308" s="2">
         <v>45338</v>
       </c>
@@ -9303,8 +9387,11 @@
       <c r="J308" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K308" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="309" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A309" s="2">
         <v>45338</v>
       </c>
@@ -9334,7 +9421,7 @@
       </c>
       <c r="J309" s="3"/>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A310" s="2">
         <v>45338</v>
       </c>
@@ -9364,7 +9451,7 @@
       </c>
       <c r="J310" s="3"/>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A311" s="2">
         <v>45338</v>
       </c>
@@ -9394,7 +9481,7 @@
       </c>
       <c r="J311" s="3"/>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A312" s="2">
         <v>45338</v>
       </c>
@@ -9424,7 +9511,7 @@
       </c>
       <c r="J312" s="3"/>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A313" s="2">
         <v>45338</v>
       </c>
@@ -9454,7 +9541,7 @@
       </c>
       <c r="J313" s="3"/>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A314" s="2">
         <v>45338</v>
       </c>
@@ -9484,7 +9571,7 @@
       </c>
       <c r="J314" s="3"/>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A315" s="2">
         <v>45338</v>
       </c>
@@ -9514,7 +9601,7 @@
       </c>
       <c r="J315" s="3"/>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A316" s="2">
         <v>45338</v>
       </c>
@@ -9540,7 +9627,7 @@
       </c>
       <c r="J316" s="3"/>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A317" s="2">
         <v>45338</v>
       </c>
@@ -9566,7 +9653,7 @@
       </c>
       <c r="J317" s="3"/>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A318" s="2">
         <v>45338</v>
       </c>
@@ -9592,7 +9679,7 @@
       </c>
       <c r="J318" s="3"/>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A319" s="2">
         <v>45338</v>
       </c>
@@ -9618,7 +9705,7 @@
       </c>
       <c r="J319" s="3"/>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A320" s="2">
         <v>45338</v>
       </c>
@@ -9644,7 +9731,7 @@
       </c>
       <c r="J320" s="3"/>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A321" s="2">
         <v>45338</v>
       </c>
@@ -9670,7 +9757,7 @@
       </c>
       <c r="J321" s="3"/>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A322" s="2">
         <v>45338</v>
       </c>
@@ -9696,7 +9783,7 @@
       </c>
       <c r="J322" s="3"/>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A323" s="2">
         <v>45339</v>
       </c>
@@ -9728,7 +9815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A324" s="2">
         <v>45339</v>
       </c>
@@ -9760,7 +9847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A325" s="2">
         <v>45339</v>
       </c>
@@ -9792,7 +9879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A326" s="2">
         <v>45339</v>
       </c>
@@ -9824,7 +9911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A327" s="2">
         <v>45339</v>
       </c>
@@ -9856,7 +9943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A328" s="2">
         <v>45339</v>
       </c>
@@ -9887,8 +9974,11 @@
       <c r="J328" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K328" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="329" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A329" s="2">
         <v>45339</v>
       </c>
@@ -9919,8 +10009,11 @@
       <c r="J329" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K329" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="330" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A330" s="2">
         <v>45339</v>
       </c>
@@ -9950,7 +10043,7 @@
       </c>
       <c r="J330" s="3"/>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A331" s="2">
         <v>45339</v>
       </c>
@@ -9980,7 +10073,7 @@
       </c>
       <c r="J331" s="3"/>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A332" s="2">
         <v>45339</v>
       </c>
@@ -10010,7 +10103,7 @@
       </c>
       <c r="J332" s="3"/>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A333" s="2">
         <v>45339</v>
       </c>
@@ -10040,7 +10133,7 @@
       </c>
       <c r="J333" s="3"/>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A334" s="2">
         <v>45339</v>
       </c>
@@ -10070,7 +10163,7 @@
       </c>
       <c r="J334" s="3"/>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A335" s="2">
         <v>45339</v>
       </c>
@@ -10100,7 +10193,7 @@
       </c>
       <c r="J335" s="3"/>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A336" s="2">
         <v>45339</v>
       </c>
@@ -10130,7 +10223,7 @@
       </c>
       <c r="J336" s="3"/>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A337" s="2">
         <v>45339</v>
       </c>
@@ -10162,7 +10255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A338" s="2">
         <v>45339</v>
       </c>
@@ -10194,7 +10287,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A339" s="2">
         <v>45339</v>
       </c>
@@ -10226,7 +10319,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A340" s="2">
         <v>45339</v>
       </c>
@@ -10258,7 +10351,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A341" s="2">
         <v>45339</v>
       </c>
@@ -10290,7 +10383,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A342" s="2">
         <v>45339</v>
       </c>
@@ -10321,8 +10414,11 @@
       <c r="J342" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K342" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="343" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A343" s="2">
         <v>45339</v>
       </c>
@@ -10353,8 +10449,11 @@
       <c r="J343" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K343" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="344" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A344" s="2">
         <v>45339</v>
       </c>
@@ -10384,7 +10483,7 @@
       </c>
       <c r="J344" s="3"/>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A345" s="2">
         <v>45339</v>
       </c>
@@ -10414,7 +10513,7 @@
       </c>
       <c r="J345" s="3"/>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A346" s="2">
         <v>45339</v>
       </c>
@@ -10444,7 +10543,7 @@
       </c>
       <c r="J346" s="3"/>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A347" s="2">
         <v>45339</v>
       </c>
@@ -10474,7 +10573,7 @@
       </c>
       <c r="J347" s="3"/>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A348" s="2">
         <v>45339</v>
       </c>
@@ -10504,7 +10603,7 @@
       </c>
       <c r="J348" s="3"/>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A349" s="2">
         <v>45339</v>
       </c>
@@ -10534,7 +10633,7 @@
       </c>
       <c r="J349" s="3"/>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A350" s="2">
         <v>45339</v>
       </c>
@@ -10564,7 +10663,7 @@
       </c>
       <c r="J350" s="3"/>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A351" s="2">
         <v>45339</v>
       </c>
@@ -10590,7 +10689,7 @@
       </c>
       <c r="J351" s="3"/>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A352" s="2">
         <v>45339</v>
       </c>
@@ -10616,7 +10715,7 @@
       </c>
       <c r="J352" s="3"/>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A353" s="2">
         <v>45339</v>
       </c>
@@ -10642,7 +10741,7 @@
       </c>
       <c r="J353" s="3"/>
     </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A354" s="2">
         <v>45339</v>
       </c>
@@ -10668,7 +10767,7 @@
       </c>
       <c r="J354" s="3"/>
     </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A355" s="2">
         <v>45339</v>
       </c>
@@ -10694,7 +10793,7 @@
       </c>
       <c r="J355" s="3"/>
     </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A356" s="2">
         <v>45339</v>
       </c>
@@ -10720,7 +10819,7 @@
       </c>
       <c r="J356" s="3"/>
     </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A357" s="2">
         <v>45339</v>
       </c>
@@ -10746,7 +10845,7 @@
       </c>
       <c r="J357" s="3"/>
     </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A358" s="2">
         <v>45340</v>
       </c>
@@ -10777,8 +10876,11 @@
       <c r="J358" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K358" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="359" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A359" s="2">
         <v>45340</v>
       </c>
@@ -10810,7 +10912,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="360" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A360" s="2">
         <v>45340</v>
       </c>
@@ -10842,7 +10944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A361" s="2">
         <v>45340</v>
       </c>
@@ -10874,7 +10976,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A362" s="2">
         <v>45340</v>
       </c>
@@ -10906,7 +11008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A363" s="2">
         <v>45340</v>
       </c>
@@ -10938,7 +11040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A364" s="2">
         <v>45340</v>
       </c>
@@ -10969,8 +11071,11 @@
       <c r="J364" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K364" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="365" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A365" s="2">
         <v>45340</v>
       </c>
@@ -11000,7 +11105,7 @@
       </c>
       <c r="J365" s="3"/>
     </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A366" s="2">
         <v>45340</v>
       </c>
@@ -11030,7 +11135,7 @@
       </c>
       <c r="J366" s="3"/>
     </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A367" s="2">
         <v>45340</v>
       </c>
@@ -11060,7 +11165,7 @@
       </c>
       <c r="J367" s="3"/>
     </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A368" s="2">
         <v>45340</v>
       </c>
@@ -11307,6 +11412,9 @@
       <c r="J375" s="3">
         <v>5</v>
       </c>
+      <c r="K375" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="376" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A376" s="2">
@@ -11406,6 +11514,9 @@
       <c r="J378" s="3">
         <v>4</v>
       </c>
+      <c r="K378" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="379" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A379" s="2">
@@ -11587,7 +11698,7 @@
       </c>
       <c r="J384" s="3"/>
     </row>
-    <row r="385" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A385" s="2">
         <v>45340</v>
       </c>
@@ -11617,7 +11728,7 @@
       </c>
       <c r="J385" s="3"/>
     </row>
-    <row r="386" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A386" s="2">
         <v>45340</v>
       </c>
@@ -11643,7 +11754,7 @@
       </c>
       <c r="J386" s="3"/>
     </row>
-    <row r="387" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A387" s="2">
         <v>45340</v>
       </c>
@@ -11669,7 +11780,7 @@
       </c>
       <c r="J387" s="3"/>
     </row>
-    <row r="388" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A388" s="2">
         <v>45340</v>
       </c>
@@ -11695,7 +11806,7 @@
       </c>
       <c r="J388" s="3"/>
     </row>
-    <row r="389" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A389" s="2">
         <v>45340</v>
       </c>
@@ -11721,7 +11832,7 @@
       </c>
       <c r="J389" s="3"/>
     </row>
-    <row r="390" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A390" s="2">
         <v>45340</v>
       </c>
@@ -11747,7 +11858,7 @@
       </c>
       <c r="J390" s="3"/>
     </row>
-    <row r="391" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A391" s="2">
         <v>45340</v>
       </c>
@@ -11773,7 +11884,7 @@
       </c>
       <c r="J391" s="3"/>
     </row>
-    <row r="392" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A392" s="2">
         <v>45340</v>
       </c>
@@ -11799,7 +11910,7 @@
       </c>
       <c r="J392" s="3"/>
     </row>
-    <row r="393" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A393" s="2">
         <v>45341</v>
       </c>
@@ -11831,7 +11942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="394" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A394" s="2">
         <v>45341</v>
       </c>
@@ -11862,8 +11973,11 @@
       <c r="J394" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="395" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K394" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="395" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A395" s="2">
         <v>45341</v>
       </c>
@@ -11895,7 +12009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="396" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A396" s="2">
         <v>45341</v>
       </c>
@@ -11926,8 +12040,11 @@
       <c r="J396" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="397" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K396" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="397" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A397" s="2">
         <v>45341</v>
       </c>
@@ -11959,7 +12076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="398" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A398" s="2">
         <v>45341</v>
       </c>
@@ -11991,7 +12108,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="399" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A399" s="2">
         <v>45341</v>
       </c>
@@ -12023,7 +12140,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="400" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A400" s="2">
         <v>45341</v>
       </c>
@@ -12264,6 +12381,9 @@
       <c r="J407" s="3">
         <v>4</v>
       </c>
+      <c r="K407" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="408" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A408" s="2">
@@ -12296,6 +12416,9 @@
       <c r="J408" s="3">
         <v>4</v>
       </c>
+      <c r="K408" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="409" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A409" s="2">
@@ -12360,6 +12483,9 @@
       <c r="J410" s="3">
         <v>4</v>
       </c>
+      <c r="K410" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="411" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A411" s="2">
@@ -12550,7 +12676,7 @@
       </c>
       <c r="J416" s="3"/>
     </row>
-    <row r="417" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A417" s="2">
         <v>45341</v>
       </c>
@@ -12580,7 +12706,7 @@
       </c>
       <c r="J417" s="3"/>
     </row>
-    <row r="418" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A418" s="2">
         <v>45341</v>
       </c>
@@ -12610,7 +12736,7 @@
       </c>
       <c r="J418" s="3"/>
     </row>
-    <row r="419" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A419" s="2">
         <v>45341</v>
       </c>
@@ -12640,7 +12766,7 @@
       </c>
       <c r="J419" s="3"/>
     </row>
-    <row r="420" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A420" s="2">
         <v>45341</v>
       </c>
@@ -12670,7 +12796,7 @@
       </c>
       <c r="J420" s="3"/>
     </row>
-    <row r="421" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A421" s="2">
         <v>45341</v>
       </c>
@@ -12696,7 +12822,7 @@
       </c>
       <c r="J421" s="3"/>
     </row>
-    <row r="422" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A422" s="2">
         <v>45341</v>
       </c>
@@ -12722,7 +12848,7 @@
       </c>
       <c r="J422" s="3"/>
     </row>
-    <row r="423" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A423" s="2">
         <v>45341</v>
       </c>
@@ -12748,7 +12874,7 @@
       </c>
       <c r="J423" s="3"/>
     </row>
-    <row r="424" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A424" s="2">
         <v>45341</v>
       </c>
@@ -12774,7 +12900,7 @@
       </c>
       <c r="J424" s="3"/>
     </row>
-    <row r="425" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A425" s="2">
         <v>45341</v>
       </c>
@@ -12800,7 +12926,7 @@
       </c>
       <c r="J425" s="3"/>
     </row>
-    <row r="426" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A426" s="2">
         <v>45341</v>
       </c>
@@ -12826,7 +12952,7 @@
       </c>
       <c r="J426" s="3"/>
     </row>
-    <row r="427" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A427" s="2">
         <v>45341</v>
       </c>
@@ -12852,7 +12978,7 @@
       </c>
       <c r="J427" s="3"/>
     </row>
-    <row r="428" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A428" s="2">
         <v>45342</v>
       </c>
@@ -12884,7 +13010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="429" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A429" s="2">
         <v>45342</v>
       </c>
@@ -12916,7 +13042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="430" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A430" s="2">
         <v>45342</v>
       </c>
@@ -12947,8 +13073,11 @@
       <c r="J430" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="431" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K430" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="431" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A431" s="2">
         <v>45342</v>
       </c>
@@ -12980,7 +13109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="432" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A432" s="2">
         <v>45342</v>
       </c>
@@ -13012,7 +13141,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="433" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A433" s="2">
         <v>45342</v>
       </c>
@@ -13043,8 +13172,11 @@
       <c r="J433" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="434" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K433" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="434" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A434" s="2">
         <v>45342</v>
       </c>
@@ -13076,7 +13208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="435" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A435" s="2">
         <v>45342</v>
       </c>
@@ -13106,7 +13238,7 @@
       </c>
       <c r="J435" s="3"/>
     </row>
-    <row r="436" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A436" s="2">
         <v>45342</v>
       </c>
@@ -13136,7 +13268,7 @@
       </c>
       <c r="J436" s="3"/>
     </row>
-    <row r="437" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A437" s="2">
         <v>45342</v>
       </c>
@@ -13166,7 +13298,7 @@
       </c>
       <c r="J437" s="3"/>
     </row>
-    <row r="438" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A438" s="2">
         <v>45342</v>
       </c>
@@ -13196,7 +13328,7 @@
       </c>
       <c r="J438" s="3"/>
     </row>
-    <row r="439" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A439" s="2">
         <v>45342</v>
       </c>
@@ -13226,7 +13358,7 @@
       </c>
       <c r="J439" s="3"/>
     </row>
-    <row r="440" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A440" s="2">
         <v>45342</v>
       </c>
@@ -13256,7 +13388,7 @@
       </c>
       <c r="J440" s="3"/>
     </row>
-    <row r="441" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A441" s="2">
         <v>45342</v>
       </c>
@@ -13286,7 +13418,7 @@
       </c>
       <c r="J441" s="3"/>
     </row>
-    <row r="442" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A442" s="2">
         <v>45342</v>
       </c>
@@ -13318,7 +13450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="443" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A443" s="2">
         <v>45342</v>
       </c>
@@ -13349,8 +13481,11 @@
       <c r="J443" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="444" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K443" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="444" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A444" s="2">
         <v>45342</v>
       </c>
@@ -13381,8 +13516,11 @@
       <c r="J444" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="445" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K444" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="445" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A445" s="2">
         <v>45342</v>
       </c>
@@ -13414,7 +13552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="446" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A446" s="2">
         <v>45342</v>
       </c>
@@ -13446,7 +13584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="447" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A447" s="2">
         <v>45342</v>
       </c>
@@ -13478,7 +13616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="448" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A448" s="2">
         <v>45342</v>
       </c>
@@ -13510,7 +13648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="449" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A449" s="2">
         <v>45342</v>
       </c>
@@ -13540,7 +13678,7 @@
       </c>
       <c r="J449" s="3"/>
     </row>
-    <row r="450" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A450" s="2">
         <v>45342</v>
       </c>
@@ -13570,7 +13708,7 @@
       </c>
       <c r="J450" s="3"/>
     </row>
-    <row r="451" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A451" s="2">
         <v>45342</v>
       </c>
@@ -13600,7 +13738,7 @@
       </c>
       <c r="J451" s="3"/>
     </row>
-    <row r="452" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A452" s="2">
         <v>45342</v>
       </c>
@@ -13630,7 +13768,7 @@
       </c>
       <c r="J452" s="3"/>
     </row>
-    <row r="453" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A453" s="2">
         <v>45342</v>
       </c>
@@ -13660,7 +13798,7 @@
       </c>
       <c r="J453" s="3"/>
     </row>
-    <row r="454" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A454" s="2">
         <v>45342</v>
       </c>
@@ -13690,7 +13828,7 @@
       </c>
       <c r="J454" s="3"/>
     </row>
-    <row r="455" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A455" s="2">
         <v>45342</v>
       </c>
@@ -13720,7 +13858,7 @@
       </c>
       <c r="J455" s="3"/>
     </row>
-    <row r="456" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A456" s="2">
         <v>45342</v>
       </c>
@@ -13746,7 +13884,7 @@
       </c>
       <c r="J456" s="3"/>
     </row>
-    <row r="457" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A457" s="2">
         <v>45342</v>
       </c>
@@ -13772,7 +13910,7 @@
       </c>
       <c r="J457" s="3"/>
     </row>
-    <row r="458" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A458" s="2">
         <v>45342</v>
       </c>
@@ -13798,7 +13936,7 @@
       </c>
       <c r="J458" s="3"/>
     </row>
-    <row r="459" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A459" s="2">
         <v>45342</v>
       </c>
@@ -13824,7 +13962,7 @@
       </c>
       <c r="J459" s="3"/>
     </row>
-    <row r="460" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A460" s="2">
         <v>45342</v>
       </c>
@@ -13850,7 +13988,7 @@
       </c>
       <c r="J460" s="3"/>
     </row>
-    <row r="461" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A461" s="2">
         <v>45342</v>
       </c>
@@ -13876,7 +14014,7 @@
       </c>
       <c r="J461" s="3"/>
     </row>
-    <row r="462" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A462" s="2">
         <v>45342</v>
       </c>
@@ -13902,7 +14040,7 @@
       </c>
       <c r="J462" s="3"/>
     </row>
-    <row r="463" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A463" s="2">
         <v>45343</v>
       </c>
@@ -13933,8 +14071,11 @@
       <c r="J463" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="464" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K463" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="464" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A464" s="2">
         <v>45343</v>
       </c>
@@ -13966,7 +14107,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="465" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A465" s="2">
         <v>45343</v>
       </c>
@@ -13998,7 +14139,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="466" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A466" s="2">
         <v>45343</v>
       </c>
@@ -14029,8 +14170,11 @@
       <c r="J466" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="467" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K466" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="467" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A467" s="2">
         <v>45343</v>
       </c>
@@ -14062,7 +14206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="468" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A468" s="2">
         <v>45343</v>
       </c>
@@ -14094,7 +14238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="469" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A469" s="2">
         <v>45343</v>
       </c>
@@ -14126,7 +14270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="470" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A470" s="2">
         <v>45343</v>
       </c>
@@ -14156,7 +14300,7 @@
       </c>
       <c r="J470" s="3"/>
     </row>
-    <row r="471" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A471" s="2">
         <v>45343</v>
       </c>
@@ -14186,7 +14330,7 @@
       </c>
       <c r="J471" s="3"/>
     </row>
-    <row r="472" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A472" s="2">
         <v>45343</v>
       </c>
@@ -14216,7 +14360,7 @@
       </c>
       <c r="J472" s="3"/>
     </row>
-    <row r="473" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A473" s="2">
         <v>45343</v>
       </c>
@@ -14246,7 +14390,7 @@
       </c>
       <c r="J473" s="3"/>
     </row>
-    <row r="474" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A474" s="2">
         <v>45343</v>
       </c>
@@ -14276,7 +14420,7 @@
       </c>
       <c r="J474" s="3"/>
     </row>
-    <row r="475" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A475" s="2">
         <v>45343</v>
       </c>
@@ -14306,7 +14450,7 @@
       </c>
       <c r="J475" s="3"/>
     </row>
-    <row r="476" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A476" s="2">
         <v>45343</v>
       </c>
@@ -14336,7 +14480,7 @@
       </c>
       <c r="J476" s="3"/>
     </row>
-    <row r="477" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A477" s="2">
         <v>45343</v>
       </c>
@@ -14368,7 +14512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="478" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A478" s="2">
         <v>45343</v>
       </c>
@@ -14399,8 +14543,11 @@
       <c r="J478" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="479" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K478" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="479" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A479" s="2">
         <v>45343</v>
       </c>
@@ -14431,8 +14578,11 @@
       <c r="J479" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="480" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K479" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="480" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A480" s="2">
         <v>45343</v>
       </c>

</xml_diff>